<commit_message>
Changes added for distributions paper: (i) Fix to C1 fraction made it production weighted (ii) Code to remove large clusters in Alvarez dataset, (iii) Fix to methane slip adder to site level results, (iv) minor cleanup
</commit_message>
<xml_diff>
--- a/OPGEEProxyCH4Version/OPGEE_2tranche_table_weights.xlsx
+++ b/OPGEEProxyCH4Version/OPGEE_2tranche_table_weights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruthe\Dropbox\Doctoral\Projects\Research Projects\OPGEE\0_OPGEE_Matlab\Version 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruthe\BU_methane_model\OPGEEProxyCH4Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B693CAD1-CC5B-413D-8D74-CC8CCB589B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD9CDF1-7473-4557-B640-B36198112AEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Oil bins</t>
   </si>
@@ -35,12 +35,38 @@
   <si>
     <t>normalize to smallest</t>
   </si>
+  <si>
+    <t>Total gas (Mscf/day)</t>
+  </si>
+  <si>
+    <r>
+      <t>Total oil production (bbl/day</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +201,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +394,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -472,6 +516,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -518,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -526,6 +581,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -848,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,6 +1282,165 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f>A3+I3</f>
+        <v>245895</v>
+      </c>
+      <c r="C16" s="1">
+        <f>C3+K3</f>
+        <v>76109</v>
+      </c>
+      <c r="D16" s="1">
+        <f>D3+L3</f>
+        <v>271261.24249999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" ref="A17:A26" si="0">A4+I4</f>
+        <v>194788</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" ref="C17:D17" si="1">C4+K4</f>
+        <v>501550</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>588269.17200000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>93559</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:D18" si="2">C5+K5</f>
+        <v>676320</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>316071.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>101454</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" ref="C19:D19" si="3">C6+K6</f>
+        <v>1466670</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="3"/>
+        <v>376915.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>143749</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:D20" si="4">C7+K7</f>
+        <v>4693300</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="4"/>
+        <v>659922.80000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>90800</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21:D21" si="5">C8+K8</f>
+        <v>6412300</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="5"/>
+        <v>894239.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>104372</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" ref="C22:D22" si="6">C9+K9</f>
+        <v>22436200</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="6"/>
+        <v>2759235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>17102</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" ref="C23:D23" si="7">C10+K10</f>
+        <v>11803100</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="7"/>
+        <v>963717.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>13023</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:D24" si="8">C11+K11</f>
+        <v>31368200</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="8"/>
+        <v>696325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>457</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:D25" si="9">C12+K12</f>
+        <v>7435100</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="9"/>
+        <v>100777.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="C26" s="1">
+        <f>SUM(C16:C25)*365/1000000</f>
+        <v>31707.129884999998</v>
+      </c>
+      <c r="D26" s="1">
+        <f>SUM(D16:D25)*365/1000000</f>
+        <v>2783.7580430424996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>